<commit_message>
adapt code to barcoded expeditions
</commit_message>
<xml_diff>
--- a/input/matK_rbcL_trnh_ITS_12samples_publicationsummer2022_9Qiagen_3MN/Description_sample.xlsx
+++ b/input/matK_rbcL_trnh_ITS_12samples_publicationsummer2022_9Qiagen_3MN/Description_sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\ghassan_unix\genorobotics\run-pipeline\input\matK_rbcL_trnh_ITS_12samples_publicationsummer2022_9Qiagen_3MN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AF49BB-4DF8-4C11-9CCD-D7310B71D8B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ADCEFC-2B61-4FD3-9265-AA5D3A551840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="15943" activeTab="3" xr2:uid="{C6D31C33-8899-4988-9499-3F32E6A125F8}"/>
   </bookViews>
@@ -39,56 +39,113 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>ref</t>
   </si>
   <si>
+    <t>experiment</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Barcode sequences</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>trnH-psbA</t>
+  </si>
+  <si>
+    <t>ITS</t>
+  </si>
+  <si>
+    <t>rbcL</t>
+  </si>
+  <si>
+    <t>matk</t>
+  </si>
+  <si>
+    <t>fwd</t>
+  </si>
+  <si>
+    <t>rev</t>
+  </si>
+  <si>
+    <t>CCC RTY CAT CTG GAA ATC TTG GTT C</t>
+  </si>
+  <si>
+    <t>GCT RTR ATA ATG AGA AAG ATT TCT GC</t>
+  </si>
+  <si>
+    <t>ATG TCA CCA CAA ACA GAG ACT AAA GC</t>
+  </si>
+  <si>
+    <t>TCG CAT GTA CCT GCA GTA GC</t>
+  </si>
+  <si>
+    <t>CGC GCA TGG TGG ATT CAC AAT</t>
+  </si>
+  <si>
+    <t>GTT ATG CAT GAA CGT AAT GCT</t>
+  </si>
+  <si>
+    <t>CCT TAT CAY TTA GAG GAA GGA</t>
+  </si>
+  <si>
+    <t>CCG CTT AKT GAT ATG CTT AAA</t>
+  </si>
+  <si>
+    <t>Barcode number</t>
+  </si>
+  <si>
+    <t>literature source</t>
+  </si>
+  <si>
+    <t>Yu et al.(2011)</t>
+  </si>
+  <si>
+    <t>Kress and Erickson (2007) for forward and Fay et al. (1997) for reverse</t>
+  </si>
+  <si>
+    <t>CC Tate (2002) for rev and Sang et al. (1997) for fwd</t>
+  </si>
+  <si>
+    <t>G Cheng et al. (2016)</t>
+  </si>
+  <si>
+    <t>gene</t>
+  </si>
+  <si>
+    <t>Volume(ml)</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
     <t>Prunelle project</t>
   </si>
   <si>
-    <t>experiment</t>
-  </si>
-  <si>
     <t>Sequencing of Qiagen samples without purification</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
     <t>DNA extracted with Qiagen DNeasy kit (high quality DNA), amplified by PCR to amplify matK, rbcL, trnH-psbA, ITS on 12 different plants, library prep &amp; sequencing done with: rapid sequencing kit-barcoding (SQK-RBK004) &amp; minIon flowcell</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
-    <t>Barcode sequences</t>
-  </si>
-  <si>
-    <t>unknown</t>
-  </si>
-  <si>
-    <t>Samples</t>
-  </si>
-  <si>
-    <t>Species</t>
-  </si>
-  <si>
-    <t>Matk</t>
-  </si>
-  <si>
-    <t>trnH-psbA</t>
-  </si>
-  <si>
-    <t>ITS</t>
-  </si>
-  <si>
-    <t>rbcL</t>
-  </si>
-  <si>
     <t>Ailanthus altissima</t>
   </si>
   <si>
@@ -125,40 +182,16 @@
     <t>Hedera helix</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>matk</t>
-  </si>
-  <si>
-    <t>fwd</t>
-  </si>
-  <si>
-    <t>rev</t>
-  </si>
-  <si>
-    <t>CCC RTY CAT CTG GAA ATC TTG GTT C</t>
-  </si>
-  <si>
-    <t>GCT RTR ATA ATG AGA AAG ATT TCT GC</t>
-  </si>
-  <si>
-    <t>ATG TCA CCA CAA ACA GAG ACT AAA GC</t>
-  </si>
-  <si>
-    <t>TCG CAT GTA CCT GCA GTA GC</t>
-  </si>
-  <si>
-    <t>CGC GCA TGG TGG ATT CAC AAT</t>
-  </si>
-  <si>
-    <t>GTT ATG CAT GAA CGT AAT GCT</t>
-  </si>
-  <si>
-    <t>CCT TAT CAY TTA GAG GAA GGA</t>
-  </si>
-  <si>
-    <t>CCG CTT AKT GAT ATG CTT AAA</t>
+    <t>rbcL, trnH-psbA</t>
+  </si>
+  <si>
+    <t>matK, rbcL, trnH-psbA, ITS</t>
+  </si>
+  <si>
+    <t>rbcL, trnH-psbA, ITS</t>
+  </si>
+  <si>
+    <t>matK, rbcL, ITS</t>
   </si>
 </sst>
 </file>
@@ -540,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663BC97E-857E-415F-99D9-051B5EAA442E}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -554,35 +587,32 @@
     <col min="4" max="4" width="38.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="153.44999999999999" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>0</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="153.44999999999999" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -595,14 +625,21 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="19.3046875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -610,7 +647,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.4">
@@ -618,7 +655,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.4">
@@ -626,7 +663,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.4">
@@ -634,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
@@ -642,7 +679,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
@@ -650,7 +687,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.4">
@@ -658,7 +695,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.4">
@@ -666,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.4">
@@ -674,7 +711,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.4">
@@ -682,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.4">
@@ -690,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.4">
@@ -698,7 +735,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.4">
@@ -706,7 +743,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.4">
@@ -714,7 +751,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -724,251 +761,203 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAF21846-4609-4B1F-A61C-BC04D55A3D42}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="32.3828125" customWidth="1"/>
+    <col min="4" max="4" width="16.765625" customWidth="1"/>
+    <col min="5" max="5" width="12.53515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="D5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+        <v>48</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+        <v>44</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+        <v>50</v>
+      </c>
+      <c r="D12">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>28</v>
+        <v>48</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -978,68 +967,85 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8C4E26-C426-4B60-93EE-291ACF656594}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="39.921875" customWidth="1"/>
-    <col min="3" max="3" width="29.53515625" customWidth="1"/>
+    <col min="1" max="1" width="13.53515625" customWidth="1"/>
+    <col min="2" max="2" width="43.61328125" customWidth="1"/>
+    <col min="3" max="3" width="36.07421875" customWidth="1"/>
+    <col min="4" max="4" width="24.921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
       <c r="C3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>